<commit_message>
Completed assignments on EOQ , Kanban , Safety Stocks
</commit_message>
<xml_diff>
--- a/Supply-Chain-Management/Economic_order_inventory.xlsx
+++ b/Supply-Chain-Management/Economic_order_inventory.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maluc\OneDrive\Desktop\Git\Notes\Supply-Chain-Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26e234d50582f689/Desktop/Git/Notes/Supply-Chain-Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{5FA06AFB-9A66-42E6-99A7-D9723385E794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F6D6BD5A-B538-4114-B622-573D800792B3}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{5FA06AFB-9A66-42E6-99A7-D9723385E794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0E06DBD5-C520-446B-B99D-F70EAF0809A3}"/>
   <bookViews>
-    <workbookView xWindow="4088" yWindow="16702" windowWidth="20715" windowHeight="13276" xr2:uid="{916C4053-F8DD-4078-9264-00135AF32A5A}"/>
+    <workbookView xWindow="4088" yWindow="16702" windowWidth="20715" windowHeight="13276" activeTab="4" xr2:uid="{916C4053-F8DD-4078-9264-00135AF32A5A}"/>
   </bookViews>
   <sheets>
     <sheet name="EOI" sheetId="1" r:id="rId1"/>
     <sheet name="Safety Stock" sheetId="2" r:id="rId2"/>
+    <sheet name="Lecture Safety Stock" sheetId="3" r:id="rId3"/>
+    <sheet name="Kanban" sheetId="4" r:id="rId4"/>
+    <sheet name="Quiz Safety Stock Data" sheetId="5" r:id="rId5"/>
+    <sheet name="EOQ" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>Product Value</t>
   </si>
@@ -57,15 +61,95 @@
   <si>
     <t>Total Cost</t>
   </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Calculating the safety stock</t>
+  </si>
+  <si>
+    <t>Average Demand</t>
+  </si>
+  <si>
+    <t>Order Lead Time</t>
+  </si>
+  <si>
+    <t>Standard Deviation of Demand</t>
+  </si>
+  <si>
+    <t>Average Lead Time</t>
+  </si>
+  <si>
+    <t>Standard Deviation of Lead Time</t>
+  </si>
+  <si>
+    <t>Sc</t>
+  </si>
+  <si>
+    <t>Service Lvl(Prcentage)</t>
+  </si>
+  <si>
+    <t>Service Level(k)</t>
+  </si>
+  <si>
+    <t>SS = k*Sc</t>
+  </si>
+  <si>
+    <t>Safety Stock</t>
+  </si>
+  <si>
+    <t>Product A</t>
+  </si>
+  <si>
+    <t>Product B</t>
+  </si>
+  <si>
+    <t>Product C</t>
+  </si>
+  <si>
+    <t>Product D</t>
+  </si>
+  <si>
+    <t>Product E</t>
+  </si>
+  <si>
+    <t>EOQ</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>OC</t>
+  </si>
+  <si>
+    <t>Holding Cost</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>Kanban</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="170" formatCode="&quot;₹&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,16 +165,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -98,15 +217,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE0E0E0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE0E0E0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE0E0E0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE0E0E0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,6 +671,407 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Lecture Safety Stock'!$H$17:$N$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>57.722093172362712</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61.436022552149403</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.001826611708395</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.071267637254607</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.392395176898233</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>108.44410358352599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>130.5097381101867</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FC0D-4FAB-98D7-6B65E3000A62}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="528796815"/>
+        <c:axId val="244118143"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="528796815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="244118143"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="244118143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528796815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -559,6 +1112,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1070,6 +1660,557 @@
       <a:ln>
         <a:noFill/>
       </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
@@ -1096,6 +2237,135 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08BBD08D-6BA4-4FFF-82D3-8C00F9CCD871}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>110458</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>273409</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>170208</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA02902B-D9CE-4F2A-98F0-F87BDA572002}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5986463" y="2710783"/>
+          <a:ext cx="5274034" cy="5074663"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>614892</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>112712</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>291743</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>36511</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1B5BD6A-D82C-478F-B4AD-12A42A28128F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="614892" y="5870575"/>
+          <a:ext cx="5025139" cy="4381499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76993</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>60326</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>169068</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>20638</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39AFFBDB-874F-4DAA-BDF5-79AF6FF7A829}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1415,8 +2685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B9EC241-B080-4614-A96F-39BD9F37FF37}">
   <dimension ref="A4:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1806,4 +3076,1886 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F5F922-FC59-4A55-99AA-BBD6A570C741}">
+  <dimension ref="A1:P31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <f ca="1">RANDBETWEEN(10,30)</f>
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f t="shared" ref="A3:A31" ca="1" si="0">RANDBETWEEN(10,30)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <f ca="1">AVERAGE(A2:A31)</f>
+        <v>20.866666666666667</v>
+      </c>
+      <c r="I4" s="4">
+        <f ca="1">H4</f>
+        <v>20.866666666666667</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" ref="J4:N4" ca="1" si="1">I4</f>
+        <v>20.866666666666667</v>
+      </c>
+      <c r="K4" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>20.866666666666667</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>20.866666666666667</v>
+      </c>
+      <c r="M4" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>20.866666666666667</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>20.866666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4">
+        <f ca="1">STDEV(A2:A31)</f>
+        <v>6.5691721691934495</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" ref="I5:N7" ca="1" si="2">H5</f>
+        <v>6.5691721691934495</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.5691721691934495</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.5691721691934495</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.5691721691934495</v>
+      </c>
+      <c r="M5" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.5691721691934495</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.5691721691934495</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="4">
+        <f>AVERAGE(B2:B31)</f>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="2"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="2"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="2"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="2"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="M6" s="4">
+        <f t="shared" si="2"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="2"/>
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="4">
+        <f>STDEV(B2:B31)</f>
+        <v>1.5055453054181624</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="2"/>
+        <v>1.5055453054181624</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="2"/>
+        <v>1.5055453054181624</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="2"/>
+        <v>1.5055453054181624</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="2"/>
+        <v>1.5055453054181624</v>
+      </c>
+      <c r="M7" s="4">
+        <f t="shared" si="2"/>
+        <v>1.5055453054181624</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="2"/>
+        <v>1.5055453054181624</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <f ca="1">SQRT(H6*(H5^2) + (H4^2)*(H7^2))</f>
+        <v>35.092540896385607</v>
+      </c>
+      <c r="I9">
+        <f ca="1">SQRT(I6*(I5^2) + (I4^2)*(I7^2))</f>
+        <v>35.092540896385607</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ref="I9:N9" ca="1" si="3">SQRT(J6*(J5^2) + (J4^2)*(J7^2))</f>
+        <v>35.092540896385607</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ca="1" si="3"/>
+        <v>35.092540896385607</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ca="1" si="3"/>
+        <v>35.092540896385607</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ca="1" si="3"/>
+        <v>35.092540896385607</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ca="1" si="3"/>
+        <v>35.092540896385607</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0.995</v>
+      </c>
+      <c r="M12" s="8">
+        <v>0.999</v>
+      </c>
+      <c r="N12" s="8">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13">
+        <f>NORMSINV(H12)</f>
+        <v>1.6448536269514715</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ref="I13:N13" si="4">NORMSINV(I12)</f>
+        <v>1.7506860712521695</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>1.8807936081512504</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>2.0537489106318221</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>2.5758293035488999</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>3.0902323061678132</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>3.7190164854557084</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17">
+        <f ca="1">H13*H9</f>
+        <v>57.722093172362712</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17:N17" ca="1" si="5">I13*I9</f>
+        <v>61.436022552149403</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ca="1" si="5"/>
+        <v>66.001826611708395</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ca="1" si="5"/>
+        <v>72.071267637254607</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ca="1" si="5"/>
+        <v>90.392395176898233</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ca="1" si="5"/>
+        <v>108.44410358352599</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ca="1" si="5"/>
+        <v>130.5097381101867</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G18:G19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E222CEE-B88F-486F-8141-7EECC6C886E9}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.81640625" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <f ca="1">RANDBETWEEN(10,30)</f>
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f t="shared" ref="A3:A31" ca="1" si="0">RANDBETWEEN(10,30)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <f ca="1">AVERAGE(A2:A31)</f>
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <f>AVERAGE(B2:B31)</f>
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <f ca="1">G4*G5</f>
+        <v>114.46666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <f t="shared" ca="1" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{410C3E61-0B5F-4A72-BFC6-EEA8D2D231D9}">
+  <dimension ref="A1:W32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.1796875" customWidth="1"/>
+    <col min="13" max="13" width="20.08984375" customWidth="1"/>
+    <col min="14" max="14" width="8.90625" customWidth="1"/>
+    <col min="15" max="15" width="20.08984375" customWidth="1"/>
+    <col min="16" max="16" width="10.90625" customWidth="1"/>
+    <col min="17" max="17" width="16.54296875" customWidth="1"/>
+    <col min="19" max="19" width="14.54296875" customWidth="1"/>
+    <col min="21" max="21" width="17.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>96</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>107</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>164</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>168</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>217</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>98</v>
+      </c>
+      <c r="C4">
+        <v>94</v>
+      </c>
+      <c r="E4">
+        <v>156</v>
+      </c>
+      <c r="G4">
+        <v>200</v>
+      </c>
+      <c r="I4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="C5">
+        <v>98</v>
+      </c>
+      <c r="E5">
+        <v>161</v>
+      </c>
+      <c r="G5">
+        <v>194</v>
+      </c>
+      <c r="I5">
+        <v>184</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>97</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>155</v>
+      </c>
+      <c r="G6">
+        <v>177</v>
+      </c>
+      <c r="I6">
+        <v>196</v>
+      </c>
+      <c r="M6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S6" t="s">
+        <v>23</v>
+      </c>
+      <c r="U6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>104</v>
+      </c>
+      <c r="C7">
+        <v>95</v>
+      </c>
+      <c r="E7">
+        <v>152</v>
+      </c>
+      <c r="G7">
+        <v>172</v>
+      </c>
+      <c r="I7">
+        <v>185</v>
+      </c>
+      <c r="L7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <f>AVERAGE(A3:A32)</f>
+        <v>100.1</v>
+      </c>
+      <c r="O7">
+        <f>AVERAGE(C3:C32)</f>
+        <v>99.1</v>
+      </c>
+      <c r="Q7">
+        <f>AVERAGE(E3:E32)</f>
+        <v>156</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ref="R7:S7" si="0">AVERAGE(G3:G32)</f>
+        <v>179.86666666666667</v>
+      </c>
+      <c r="U7">
+        <f t="shared" ref="U7" si="1">AVERAGE(I3:I32)</f>
+        <v>202.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>96</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>106</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>155</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>195</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <v>208</v>
+      </c>
+      <c r="J8">
+        <v>11</v>
+      </c>
+      <c r="L8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8">
+        <f>STDEV(A3:A32)</f>
+        <v>3.0211895350832503</v>
+      </c>
+      <c r="O8">
+        <f>STDEV(C3:C32)</f>
+        <v>5.6161712322849313</v>
+      </c>
+      <c r="Q8">
+        <f>STDEV(E3:E32)</f>
+        <v>4.3151697133684568</v>
+      </c>
+      <c r="S8">
+        <f t="shared" ref="R8:S8" si="2">STDEV(G3:G32)</f>
+        <v>11.640397354674478</v>
+      </c>
+      <c r="U8">
+        <f t="shared" ref="U8" si="3">STDEV(I3:I32)</f>
+        <v>12.466091940775268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>103</v>
+      </c>
+      <c r="C9">
+        <v>102</v>
+      </c>
+      <c r="E9">
+        <v>153</v>
+      </c>
+      <c r="G9">
+        <v>193</v>
+      </c>
+      <c r="I9">
+        <v>196</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9">
+        <f>AVERAGE(B3:B32)</f>
+        <v>2.5</v>
+      </c>
+      <c r="O9">
+        <f>AVERAGE(D3:D32)</f>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="Q9">
+        <f>AVERAGE(F3:F32)</f>
+        <v>6.833333333333333</v>
+      </c>
+      <c r="S9">
+        <f t="shared" ref="R9:S9" si="4">AVERAGE(H3:H32)</f>
+        <v>8.8333333333333339</v>
+      </c>
+      <c r="U9">
+        <f t="shared" ref="U9" si="5">AVERAGE(J3:J32)</f>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>103</v>
+      </c>
+      <c r="C10">
+        <v>104</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+      <c r="G10">
+        <v>191</v>
+      </c>
+      <c r="I10">
+        <v>199</v>
+      </c>
+      <c r="L10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="4">
+        <f>STDEV(B3:B32)</f>
+        <v>0.54772255750516607</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4">
+        <f>STDEV(D3:D32)</f>
+        <v>0.40824829046386302</v>
+      </c>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4">
+        <f>STDEV(F3:F32)</f>
+        <v>0.75277265270907845</v>
+      </c>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4">
+        <f t="shared" ref="R10:S10" si="6">STDEV(H3:H32)</f>
+        <v>0.98319208025017313</v>
+      </c>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4">
+        <f t="shared" ref="U10" si="7">STDEV(J3:J32)</f>
+        <v>1.2247448713915889</v>
+      </c>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>103</v>
+      </c>
+      <c r="C11">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <v>151</v>
+      </c>
+      <c r="G11">
+        <v>182</v>
+      </c>
+      <c r="I11">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>103</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
+      </c>
+      <c r="E12">
+        <v>158</v>
+      </c>
+      <c r="G12">
+        <v>181</v>
+      </c>
+      <c r="I12">
+        <v>204</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12">
+        <f>SQRT(M9*(M8^2) + (M7^2)*(M10^2))</f>
+        <v>55.034734173222283</v>
+      </c>
+      <c r="O12">
+        <f>SQRT(O9*(O8^2) + (O7^2)*(O10^2))</f>
+        <v>42.050256603970567</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ref="Q12:S12" si="8">SQRT(Q9*(Q8^2) + (Q7^2)*(Q10^2))</f>
+        <v>117.97305361526526</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="8"/>
+        <v>180.19579267728486</v>
+      </c>
+      <c r="U12">
+        <f t="shared" ref="T12:U12" si="9">SQRT(U9*(U8^2) + (U7^2)*(U10^2))</f>
+        <v>251.10506696435337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>99</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>107</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>159</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>161</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>215</v>
+      </c>
+      <c r="J13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>103</v>
+      </c>
+      <c r="C14">
+        <v>103</v>
+      </c>
+      <c r="E14">
+        <v>154</v>
+      </c>
+      <c r="G14">
+        <v>189</v>
+      </c>
+      <c r="I14">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>90</v>
+      </c>
+      <c r="E15">
+        <v>159</v>
+      </c>
+      <c r="G15">
+        <v>171</v>
+      </c>
+      <c r="I15">
+        <v>212</v>
+      </c>
+      <c r="L15" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="8">
+        <v>0.99</v>
+      </c>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>105</v>
+      </c>
+      <c r="C16">
+        <v>104</v>
+      </c>
+      <c r="E16">
+        <v>155</v>
+      </c>
+      <c r="G16">
+        <v>174</v>
+      </c>
+      <c r="I16">
+        <v>196</v>
+      </c>
+      <c r="L16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M16">
+        <f>NORMSINV(M15)</f>
+        <v>2.3263478740408408</v>
+      </c>
+      <c r="O16">
+        <f>NORMSINV(O15)</f>
+        <v>1.9599639845400536</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" ref="Q16" si="10">NORMSINV(Q15)</f>
+        <v>1.6448536269514715</v>
+      </c>
+      <c r="S16">
+        <f t="shared" ref="S16" si="11">NORMSINV(S15)</f>
+        <v>1.6448536269514715</v>
+      </c>
+      <c r="U16">
+        <f t="shared" ref="U16" si="12">NORMSINV(U15)</f>
+        <v>1.6448536269514715</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>96</v>
+      </c>
+      <c r="C17">
+        <v>103</v>
+      </c>
+      <c r="E17">
+        <v>154</v>
+      </c>
+      <c r="G17">
+        <v>163</v>
+      </c>
+      <c r="I17">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>97</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>103</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>162</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>195</v>
+      </c>
+      <c r="H18">
+        <v>9</v>
+      </c>
+      <c r="I18">
+        <v>200</v>
+      </c>
+      <c r="J18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>103</v>
+      </c>
+      <c r="C19">
+        <v>92</v>
+      </c>
+      <c r="E19">
+        <v>158</v>
+      </c>
+      <c r="G19">
+        <v>190</v>
+      </c>
+      <c r="I19">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>100</v>
+      </c>
+      <c r="C20">
+        <v>94</v>
+      </c>
+      <c r="E20">
+        <v>164</v>
+      </c>
+      <c r="G20">
+        <v>178</v>
+      </c>
+      <c r="I20">
+        <v>213</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20">
+        <f>M16*M12</f>
+        <v>128.02993684227846</v>
+      </c>
+      <c r="O20">
+        <f>O16*O12</f>
+        <v>82.41698848444986</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" ref="Q20:S20" si="13">Q16*Q12</f>
+        <v>194.04840512160948</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="13"/>
+        <v>296.3957031466274</v>
+      </c>
+      <c r="U20">
+        <f t="shared" ref="T20:U20" si="14">U16*U12</f>
+        <v>413.03108014220879</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>102</v>
+      </c>
+      <c r="C21">
+        <v>108</v>
+      </c>
+      <c r="E21">
+        <v>158</v>
+      </c>
+      <c r="G21">
+        <v>198</v>
+      </c>
+      <c r="I21">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>100</v>
+      </c>
+      <c r="C22">
+        <v>104</v>
+      </c>
+      <c r="E22">
+        <v>154</v>
+      </c>
+      <c r="G22">
+        <v>166</v>
+      </c>
+      <c r="I22">
+        <v>208</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M22">
+        <f>M7*M9</f>
+        <v>250.25</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ref="N22:U22" si="15">N7*N9</f>
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="15"/>
+        <v>412.91666666666669</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="15"/>
+        <v>1066</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="15"/>
+        <v>1588.8222222222223</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="15"/>
+        <v>2324.15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>97</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>100</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>162</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>187</v>
+      </c>
+      <c r="H23">
+        <v>8</v>
+      </c>
+      <c r="I23">
+        <v>191</v>
+      </c>
+      <c r="J23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>99</v>
+      </c>
+      <c r="C24">
+        <v>94</v>
+      </c>
+      <c r="E24">
+        <v>159</v>
+      </c>
+      <c r="G24">
+        <v>166</v>
+      </c>
+      <c r="I24">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>95</v>
+      </c>
+      <c r="C25">
+        <v>93</v>
+      </c>
+      <c r="E25">
+        <v>152</v>
+      </c>
+      <c r="G25">
+        <v>186</v>
+      </c>
+      <c r="I25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>99</v>
+      </c>
+      <c r="C26">
+        <v>106</v>
+      </c>
+      <c r="E26">
+        <v>163</v>
+      </c>
+      <c r="G26">
+        <v>167</v>
+      </c>
+      <c r="I26">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>102</v>
+      </c>
+      <c r="C27">
+        <v>102</v>
+      </c>
+      <c r="E27">
+        <v>150</v>
+      </c>
+      <c r="G27">
+        <v>172</v>
+      </c>
+      <c r="I27">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>105</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>102</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>153</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>182</v>
+      </c>
+      <c r="H28">
+        <v>10</v>
+      </c>
+      <c r="I28">
+        <v>219</v>
+      </c>
+      <c r="J28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>100</v>
+      </c>
+      <c r="C29">
+        <v>94</v>
+      </c>
+      <c r="E29">
+        <v>154</v>
+      </c>
+      <c r="G29">
+        <v>176</v>
+      </c>
+      <c r="I29">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>96</v>
+      </c>
+      <c r="C30">
+        <v>93</v>
+      </c>
+      <c r="E30">
+        <v>153</v>
+      </c>
+      <c r="G30">
+        <v>169</v>
+      </c>
+      <c r="I30">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>101</v>
+      </c>
+      <c r="C31">
+        <v>93</v>
+      </c>
+      <c r="E31">
+        <v>152</v>
+      </c>
+      <c r="G31">
+        <v>166</v>
+      </c>
+      <c r="I31">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>98</v>
+      </c>
+      <c r="C32">
+        <v>97</v>
+      </c>
+      <c r="E32">
+        <v>150</v>
+      </c>
+      <c r="G32">
+        <v>187</v>
+      </c>
+      <c r="I32">
+        <v>202</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736136A4-2C30-48EF-A03E-23C456F1EDC4}">
+  <dimension ref="C3:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" customWidth="1"/>
+    <col min="7" max="7" width="18.08984375" customWidth="1"/>
+    <col min="8" max="8" width="15.6328125" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="3:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="10">
+        <v>75000</v>
+      </c>
+      <c r="F5" s="10">
+        <v>10000</v>
+      </c>
+      <c r="G5" s="10">
+        <v>20000</v>
+      </c>
+      <c r="H5" s="10">
+        <v>45000</v>
+      </c>
+      <c r="I5" s="10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="12">
+        <v>20</v>
+      </c>
+      <c r="F6" s="12">
+        <v>50</v>
+      </c>
+      <c r="G6" s="12">
+        <v>8000</v>
+      </c>
+      <c r="H6" s="12">
+        <v>4</v>
+      </c>
+      <c r="I6" s="12">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="12">
+        <v>30</v>
+      </c>
+      <c r="F7" s="12">
+        <v>80</v>
+      </c>
+      <c r="G7" s="12">
+        <v>300</v>
+      </c>
+      <c r="H7" s="12">
+        <v>40</v>
+      </c>
+      <c r="I7" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <f>SQRT((2*E5*E7)/(E6*E8))</f>
+        <v>1000</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:I11" si="0">SQRT((2*F5*F7)/(F6*F8))</f>
+        <v>400</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="13">
+        <f>((E5/E11)*E7)</f>
+        <v>2250</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" ref="F13:I13" si="1">((F5/F11)*F7)</f>
+        <v>2000</v>
+      </c>
+      <c r="G13" s="13">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+      <c r="H13" s="13">
+        <f>((H5/H11)*H7)</f>
+        <v>900</v>
+      </c>
+      <c r="I13" s="13">
+        <f t="shared" si="1"/>
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="13">
+        <f>(E11*E8*E6)/2</f>
+        <v>2250</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" ref="F14:I14" si="2">(F11*F8*F6)/2</f>
+        <v>2000</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" si="2"/>
+        <v>60000</v>
+      </c>
+      <c r="H14" s="13">
+        <f t="shared" si="2"/>
+        <v>900</v>
+      </c>
+      <c r="I14" s="13">
+        <f t="shared" si="2"/>
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="13">
+        <f>E13+E14</f>
+        <v>4500</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" ref="F15:I15" si="3">F13+F14</f>
+        <v>4000</v>
+      </c>
+      <c r="G15" s="13">
+        <f t="shared" si="3"/>
+        <v>120000</v>
+      </c>
+      <c r="H15" s="13">
+        <f t="shared" si="3"/>
+        <v>1800</v>
+      </c>
+      <c r="I15" s="13">
+        <f t="shared" si="3"/>
+        <v>25000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>